<commit_message>
added address decoding, interrupt handling, external bus interface
</commit_message>
<xml_diff>
--- a/docs/Bus Connector Pinouts.xlsx
+++ b/docs/Bus Connector Pinouts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/Electronics/68komputer/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12EC2FAF-3E6B-E04A-BBC3-C2E70F9836E3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3311D5-8ED5-6C45-8475-96729F2766CF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10400" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{698F115C-9D18-384A-9B16-72850D64F49E}"/>
+    <workbookView xWindow="11640" yWindow="8320" windowWidth="28040" windowHeight="17440" xr2:uid="{698F115C-9D18-384A-9B16-72850D64F49E}"/>
   </bookViews>
   <sheets>
     <sheet name="Pinouts" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="164">
   <si>
     <t>Column</t>
   </si>
@@ -188,9 +188,6 @@
   </si>
   <si>
     <t>Bus reset: asserted to reset all peripherals back into their initial states, aborting any in-progress transactions.</t>
-  </si>
-  <si>
-    <t>External Bus Interface</t>
   </si>
   <si>
     <t>Expansion Card Interface</t>
@@ -242,6 +239,308 @@
 Start mode: 00 = Read, 01 = Reserved, 10 = Write, 11 = Reserved
 Transfer mode: 00 = NACK, 01 = Reserved, 10 = bus error, 11 = Transfer complete
 IRQ acknowledge cycle: Always 00</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>A9</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>A11</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>A13</t>
+  </si>
+  <si>
+    <t>A14</t>
+  </si>
+  <si>
+    <t>A15</t>
+  </si>
+  <si>
+    <t>A16</t>
+  </si>
+  <si>
+    <t>A17</t>
+  </si>
+  <si>
+    <t>A18</t>
+  </si>
+  <si>
+    <t>A19</t>
+  </si>
+  <si>
+    <t>A20</t>
+  </si>
+  <si>
+    <t>A21</t>
+  </si>
+  <si>
+    <t>A22</t>
+  </si>
+  <si>
+    <t>A23</t>
+  </si>
+  <si>
+    <t>A24</t>
+  </si>
+  <si>
+    <t>A25</t>
+  </si>
+  <si>
+    <t>A26</t>
+  </si>
+  <si>
+    <t>A27</t>
+  </si>
+  <si>
+    <t>A28</t>
+  </si>
+  <si>
+    <t>A29</t>
+  </si>
+  <si>
+    <t>A30</t>
+  </si>
+  <si>
+    <t>A31</t>
+  </si>
+  <si>
+    <t>D0</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>D12</t>
+  </si>
+  <si>
+    <t>D13</t>
+  </si>
+  <si>
+    <t>D14</t>
+  </si>
+  <si>
+    <t>D15</t>
+  </si>
+  <si>
+    <t>D16</t>
+  </si>
+  <si>
+    <t>D17</t>
+  </si>
+  <si>
+    <t>D18</t>
+  </si>
+  <si>
+    <t>D19</t>
+  </si>
+  <si>
+    <t>D20</t>
+  </si>
+  <si>
+    <t>D21</t>
+  </si>
+  <si>
+    <t>D22</t>
+  </si>
+  <si>
+    <t>D23</t>
+  </si>
+  <si>
+    <t>D24</t>
+  </si>
+  <si>
+    <t>D25</t>
+  </si>
+  <si>
+    <t>D26</t>
+  </si>
+  <si>
+    <t>D27</t>
+  </si>
+  <si>
+    <t>D28</t>
+  </si>
+  <si>
+    <t>D29</t>
+  </si>
+  <si>
+    <t>D30</t>
+  </si>
+  <si>
+    <t>D31</t>
+  </si>
+  <si>
+    <t>/BERR</t>
+  </si>
+  <si>
+    <t>/HALT</t>
+  </si>
+  <si>
+    <t>/VPA</t>
+  </si>
+  <si>
+    <t>/BR</t>
+  </si>
+  <si>
+    <t>/BG</t>
+  </si>
+  <si>
+    <t>/BGACK</t>
+  </si>
+  <si>
+    <t>/AS</t>
+  </si>
+  <si>
+    <t>R/W</t>
+  </si>
+  <si>
+    <t>/UDS</t>
+  </si>
+  <si>
+    <t>/LDS</t>
+  </si>
+  <si>
+    <t>FC[0]</t>
+  </si>
+  <si>
+    <t>FC[1]</t>
+  </si>
+  <si>
+    <t>FC[2]</t>
+  </si>
+  <si>
+    <t>/DTACK</t>
+  </si>
+  <si>
+    <t>/IRQ</t>
+  </si>
+  <si>
+    <t>/STERM</t>
+  </si>
+  <si>
+    <t>Reserved</t>
+  </si>
+  <si>
+    <t>External Bus Interface (68000)</t>
+  </si>
+  <si>
+    <t>External Bus Interface (68030)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Reserved lines should be left floating.</t>
+    </r>
+  </si>
+  <si>
+    <t>SIZ[0]</t>
+  </si>
+  <si>
+    <t>SIZ[1]</t>
+  </si>
+  <si>
+    <t>/DS</t>
+  </si>
+  <si>
+    <t>/DSACK[0]</t>
+  </si>
+  <si>
+    <t>/DSACK[1]</t>
+  </si>
+  <si>
+    <t>/CBREQ</t>
+  </si>
+  <si>
+    <t>/RMC</t>
+  </si>
+  <si>
+    <t>/CBACK</t>
+  </si>
+  <si>
+    <t>/OCS</t>
+  </si>
+  <si>
+    <t>/ECS</t>
   </si>
 </sst>
 </file>
@@ -285,7 +584,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -311,11 +610,50 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="20">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -357,7 +695,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D0486B0-0A6D-E44F-B557-E760C375FB0D}" name="Table1" displayName="Table1" ref="B3:E35" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D0486B0-0A6D-E44F-B557-E760C375FB0D}" name="Table1" displayName="Table1" ref="B3:E35" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="B3:E35" xr:uid="{7A387C7E-0398-814F-84D8-0156A704A5DE}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -365,21 +703,52 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{88263C44-2C63-9649-B727-43EB007E08D7}" name="Column" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{C7ACD2F6-C5D0-1F49-B6E9-EDBC5E470108}" name="Row A" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{A6201D17-02F1-6B47-A869-8BCF7ACF389A}" name="Row B" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{13AFF08F-13D3-4D41-918E-020B041BC5A8}" name="Row C" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{88263C44-2C63-9649-B727-43EB007E08D7}" name="Column" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{C7ACD2F6-C5D0-1F49-B6E9-EDBC5E470108}" name="Row A" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{A6201D17-02F1-6B47-A869-8BCF7ACF389A}" name="Row B" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{13AFF08F-13D3-4D41-918E-020B041BC5A8}" name="Row C" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{49D82D6C-9B5A-CE4F-B4DB-2AD50416E3C1}" name="Table15" displayName="Table15" ref="G3:J35" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="G3:J35" xr:uid="{3C49D4B2-2802-5E4F-97A8-57E90D3F6CF0}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{AAD880CD-E3AD-3D44-9180-284FB947448B}" name="Column" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{09C6B63E-7055-BC40-8430-FBA20EBB428A}" name="Row A" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{67E6B2CE-952E-DA46-BBE5-24E2F5EA83DA}" name="Row B" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{96194A51-D007-B949-9D1B-CAC96E3E8053}" name="Row C" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B1F670F4-4104-1A4E-9CCC-2C9DA88FDC7A}" name="Table156" displayName="Table156" ref="L3:O35" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="L3:O35" xr:uid="{7E6D4E52-75D1-E641-A08E-571DE021DF11}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{BB45B602-2E92-CA43-98A8-D75DE9E7E745}" name="Column" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{7D6D4A81-AD60-F747-BAB0-CB77DE862F0C}" name="Row A" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{D1892DBF-F4FE-6B4B-A9ED-39008F05375D}" name="Row B" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{95699C5D-C37D-FF4C-9C12-0F39E11427BC}" name="Row C" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6F314FB6-EBDF-7D47-A073-19012D76BFCE}" name="Table3" displayName="Table3" ref="B3:C13" totalsRowShown="0">
   <autoFilter ref="B3:C13" xr:uid="{0DA10BB0-6F0E-C44D-A3B7-AC419D641335}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{36AF33B5-BE4A-E740-907D-402FDC7C5EED}" name="Signal" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{9B21C6BA-5CAA-D44C-B18F-371693060AB8}" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{36AF33B5-BE4A-E740-907D-402FDC7C5EED}" name="Signal" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{9B21C6BA-5CAA-D44C-B18F-371693060AB8}" name="Description" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -683,35 +1052,41 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5F35466-8B01-0D42-B321-D482E0F1EB7A}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:J35"/>
+  <dimension ref="B2:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="7" style="3" customWidth="1"/>
     <col min="3" max="5" width="10.83203125" style="1"/>
-    <col min="7" max="7" width="13.1640625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="7" style="6" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B2" s="8" t="s">
-        <v>54</v>
+        <v>151</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="G2" s="4" t="s">
-        <v>55</v>
+        <v>152</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -724,430 +1099,1251 @@
       <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="G3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B4" s="3">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L4" s="3">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B5" s="3">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="L5" s="3">
+        <v>2</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B6" s="3">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>72</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L6" s="3">
+        <v>3</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B7" s="3">
         <v>4</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
+      <c r="C7" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>5</v>
+        <v>150</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="G7" s="3">
+        <v>4</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="L7" s="3">
+        <v>4</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B8" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G8" s="3">
+        <v>5</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="L8" s="3">
+        <v>5</v>
+      </c>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B9" s="3">
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="3">
+        <v>6</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="L9" s="3">
+        <v>6</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="N9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O9" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B10" s="3">
         <v>7</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G10" s="3">
+        <v>7</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L10" s="3">
+        <v>7</v>
+      </c>
+      <c r="M10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="N10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O10" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B11" s="3">
         <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G11" s="3">
+        <v>8</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L11" s="3">
+        <v>8</v>
+      </c>
+      <c r="M11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="N11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O11" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B12" s="3">
         <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G12" s="3">
+        <v>9</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="L12" s="3">
+        <v>9</v>
+      </c>
+      <c r="M12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="N12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O12" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B13" s="3">
         <v>10</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G13" s="3">
+        <v>10</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="L13" s="3">
+        <v>10</v>
+      </c>
+      <c r="M13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="N13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O13" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B14" s="3">
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G14" s="3">
+        <v>11</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="L14" s="3">
+        <v>11</v>
+      </c>
+      <c r="M14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="N14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O14" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B15" s="3">
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G15" s="3">
+        <v>12</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L15" s="3">
+        <v>12</v>
+      </c>
+      <c r="M15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="N15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O15" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B16" s="3">
         <v>13</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G16" s="3">
+        <v>13</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="L16" s="3">
+        <v>13</v>
+      </c>
+      <c r="M16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="1" t="s">
+      <c r="N16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O16" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B17" s="3">
         <v>14</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G17" s="3">
+        <v>14</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="L17" s="3">
+        <v>14</v>
+      </c>
+      <c r="M17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="1" t="s">
+      <c r="N17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O17" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B18" s="3">
         <v>15</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G18" s="3">
+        <v>15</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L18" s="3">
+        <v>15</v>
+      </c>
+      <c r="M18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="N18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O18" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B19" s="3">
         <v>16</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G19" s="3">
+        <v>16</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L19" s="3">
+        <v>16</v>
+      </c>
+      <c r="M19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="N19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O19" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B20" s="3">
         <v>17</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G20" s="3">
+        <v>17</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="L20" s="3">
+        <v>17</v>
+      </c>
+      <c r="M20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="N20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O20" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B21" s="3">
         <v>18</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G21" s="3">
+        <v>18</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L21" s="3">
+        <v>18</v>
+      </c>
+      <c r="M21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="N21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O21" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B22" s="3">
         <v>19</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G22" s="3">
+        <v>19</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L22" s="3">
+        <v>19</v>
+      </c>
+      <c r="M22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="1" t="s">
+      <c r="N22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O22" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B23" s="3">
         <v>20</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G23" s="3">
+        <v>20</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L23" s="3">
+        <v>20</v>
+      </c>
+      <c r="M23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" s="1" t="s">
+      <c r="N23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O23" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B24" s="3">
         <v>21</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G24" s="3">
+        <v>21</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="L24" s="3">
+        <v>21</v>
+      </c>
+      <c r="M24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="1" t="s">
+      <c r="N24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O24" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B25" s="3">
         <v>22</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>5</v>
+      <c r="C25" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G25" s="3">
+        <v>22</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L25" s="3">
+        <v>22</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O25" s="1"/>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B26" s="3">
         <v>23</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>5</v>
+        <v>92</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G26" s="3">
+        <v>23</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="L26" s="3">
+        <v>23</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O26" s="1"/>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B27" s="3">
         <v>24</v>
       </c>
+      <c r="C27" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="E27" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+      <c r="G27" s="3">
+        <v>24</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="L27" s="3">
+        <v>24</v>
+      </c>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B28" s="3">
         <v>25</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G28" s="3">
+        <v>25</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="L28" s="3">
+        <v>25</v>
+      </c>
+      <c r="M28" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="N28" s="1"/>
+      <c r="O28" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B29" s="3">
         <v>26</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G29" s="3">
+        <v>26</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L29" s="3">
+        <v>26</v>
+      </c>
+      <c r="M29" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="N29" s="1"/>
+      <c r="O29" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B30" s="3">
         <v>27</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G30" s="3">
+        <v>27</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L30" s="3">
+        <v>27</v>
+      </c>
+      <c r="M30" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="N30" s="1"/>
+      <c r="O30" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B31" s="3">
         <v>28</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G31" s="3">
+        <v>28</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="L31" s="3">
+        <v>28</v>
+      </c>
+      <c r="M31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E31" s="1" t="s">
+      <c r="N31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O31" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B32" s="3">
         <v>29</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G32" s="3">
+        <v>29</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="L32" s="3">
+        <v>29</v>
+      </c>
+      <c r="M32" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="N32" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="O32" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B33" s="3">
         <v>30</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G33" s="3">
+        <v>30</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="L33" s="3">
+        <v>30</v>
+      </c>
+      <c r="M33" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="N33" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="O33" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B34" s="3">
         <v>31</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G34" s="3">
+        <v>31</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L34" s="3">
+        <v>31</v>
+      </c>
+      <c r="M34" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="N34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B35" s="3">
         <v>32</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G35" s="3">
+        <v>32</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="L35" s="3">
+        <v>32</v>
+      </c>
+      <c r="M35" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" s="1" t="s">
+      <c r="N35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O35" s="1" t="s">
         <v>25</v>
       </c>
     </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B37" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+    </row>
+    <row r="38" spans="2:15" ht="13" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="G2:J2"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="B37:J37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1194,7 +2390,7 @@
         <v>28</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="34" x14ac:dyDescent="0.2">
@@ -1202,23 +2398,23 @@
         <v>30</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="34" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="68" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="17" x14ac:dyDescent="0.2">
@@ -1226,7 +2422,7 @@
         <v>47</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="34" x14ac:dyDescent="0.2">
@@ -1234,7 +2430,7 @@
         <v>29</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="34" x14ac:dyDescent="0.2">
@@ -1242,23 +2438,23 @@
         <v>48</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added SIMM socket footprint
</commit_message>
<xml_diff>
--- a/docs/Bus Connector Pinouts.xlsx
+++ b/docs/Bus Connector Pinouts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/Electronics/68komputer/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3311D5-8ED5-6C45-8475-96729F2766CF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE17133-76C6-BA41-9711-2D454C7295FE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11640" yWindow="8320" windowWidth="28040" windowHeight="17440" xr2:uid="{698F115C-9D18-384A-9B16-72850D64F49E}"/>
+    <workbookView xWindow="-28600" yWindow="6300" windowWidth="28040" windowHeight="17440" xr2:uid="{698F115C-9D18-384A-9B16-72850D64F49E}"/>
   </bookViews>
   <sheets>
     <sheet name="Pinouts" sheetId="1" r:id="rId1"/>
@@ -1055,7 +1055,7 @@
   <dimension ref="B2:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>